<commit_message>
Task 26 and modified task 19
</commit_message>
<xml_diff>
--- a/SourceCode/2023/August2023/Deekshitha/Task 19/Data.xlsx
+++ b/SourceCode/2023/August2023/Deekshitha/Task 19/Data.xlsx
@@ -16,28 +16,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <x:si>
-    <x:t>Title</x:t>
-  </x:si>
-  <x:si>
-    <x:t>URL's</x:t>
-  </x:si>
-  <x:si>
-    <x:t>What Is Data Scraping | Techniques, Tools &amp; Mitigation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imperva.com/learn/application-security/data-scraping/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>What Is Data Scraping And How Can You Use It?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://targetinternet.com/resources/what-is-data-scraping-and-how-can-you-use-it</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Data scraping</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://en.wikipedia.org/wiki/Data_scraping</x:t>
+    <x:t>Titile Text</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title URL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>What Is Data Scraping? Definition &amp; Usage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.okta.com/identity-101/data-scraping/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>What is data scraping?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.cloudflare.com/learning/bots/what-is-data-scraping/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>What is Web Scraping and How to Use It?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.geeksforgeeks.org/what-is-web-scraping-and-how-to-use-it/</x:t>
   </x:si>
   <x:si>
     <x:t>What is Web Scraping and What is it Used For?</x:t>

</xml_diff>